<commit_message>
use material ui loader
</commit_message>
<xml_diff>
--- a/Leetcode_Approach.xlsx
+++ b/Leetcode_Approach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunwsingh/Projects/coding-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826DB39B-DC77-8A48-A82B-A6AC7302371C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15767EAA-423E-9F4A-8553-A5AF521A9BF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="410">
   <si>
     <t>Problem</t>
   </si>
@@ -2477,6 +2477,98 @@
             arr[j + 1] = key; 
         } 
     } </t>
+  </si>
+  <si>
+    <t>Reverse Nodes in k-Group</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-nodes-in-k-group/</t>
+  </si>
+  <si>
+    <t>public ListNode reverseKGroup(ListNode head, int k) {
+    ListNode begin;
+    if (head==null || head.next ==null || k==1)
+    	return head;
+    ListNode dummyhead = new ListNode(-1);
+    dummyhead.next = head;
+    begin = dummyhead;
+    int i=0;
+    while (head != null){
+    	i++;
+    	if (i%k == 0){
+    		begin = reverse(begin, head.next); 
+    		head = begin.next;
+    	} else {
+    		head = head.next;
+    	}
+    }
+    return dummyhead.next;
+}</t>
+  </si>
+  <si>
+    <t>Write a method for reverse list that accepts begin and end pointers. Return begin in reverse() as it will be the last node in the group. Also, begin will always point to the prev of the current group</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> public List&lt;int[]&gt; kSmallestPairs(int[] nums1, int[] nums2, int k) {
+        // min queue
+        PriorityQueue&lt;int[]&gt; q = new PriorityQueue&lt;&gt;((a, b) -&gt; (a[0] + a[1]) - (b[0] + b[1]));
+        List&lt;int[]&gt; res = new ArrayList();
+        int N1 = nums1.length, N2 = nums2.length;
+        if (N1 == 0 || N2 == 0) return res;
+        // offer initial pairs {num1, num2, index_of_num2}
+        for (int i = 0; i &lt; Math.min(N1, k); i++) q.offer(new int[]{nums1[i], nums2[0], 0});
+        for (int i = 0; i &lt; Math.min(N1 * N2, k); i++) {
+            int[] cur = q.poll();
+            res.add(new int[]{cur[0], cur[1]});
+            // next better pair is B: {num1, next(num2)}
+            if (cur[2] &lt; N2 - 1 ) { // boundary check
+                int idx = cur[2] + 1;
+                q.offer(new int[]{cur[0], nums2[idx], idx});
+            }
+        }
+        return res;
+    }</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-k-pairs-with-smallest-sums</t>
+  </si>
+  <si>
+    <t>Find K pairs with smallest sums</t>
+  </si>
+  <si>
+    <t>1. Take advantage of sorted lists 
+2. Create a Min Heap and add all pairs of Arr1 matched with [0] of Arr2
+3. Pop the min from heap and push to results. If results.size == k, return results;
+4. Add next element to the heap {num1, next(num2)}
+5. To keep track of next element in Arr2, also save the index from Arr2 in heap</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix</t>
+  </si>
+  <si>
+    <t>Kth Smallest Element in a Sorted Matrix</t>
+  </si>
+  <si>
+    <t>heap, binary_search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public int kthSmallest(int[][] matrix, int k) {
+        int n = matrix.length;
+        PriorityQueue&lt;Tuple&gt; pq = new PriorityQueue&lt;Tuple&gt;();
+        for(int j = 0; j &lt;= n-1; j++) pq.offer(new Tuple(0, j, matrix[0][j]));
+        for(int i = 0; i &lt; k-1; i++) {
+            Tuple t = pq.poll();
+            if(t.x &lt; n-1){
+                pq.offer(new Tuple(t.x+1, t.y, matrix[t.x+1][t.y]));
+            } 
+        }
+        return pq.poll().val;
+    }</t>
+  </si>
+  <si>
+    <t>1. Take advantage of sorted lists 
+2. Create a Min Heap and add all elements of 1st row
+3. Repeat k times: Pop the min from heap and push the next row element into heap</t>
   </si>
 </sst>
 </file>
@@ -2625,7 +2717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2683,6 +2775,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2902,10 +2995,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1032"/>
+  <dimension ref="A1:F1035"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
@@ -4001,657 +4094,687 @@
         <v>211</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="85">
-      <c r="A72" s="12" t="s">
+    <row r="72" spans="1:5" ht="285">
+      <c r="A72" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="180">
+      <c r="A73" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="E73" s="21" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="85">
+      <c r="A74" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B74" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C74" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="D74" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="E72" s="8"/>
-    </row>
-    <row r="73" spans="1:5" ht="225">
-      <c r="A73" s="5" t="s">
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" spans="1:5" ht="285">
+      <c r="A75" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="B75" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="E75" s="21" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="225">
+      <c r="A76" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B76" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D76" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="E73" s="8"/>
-    </row>
-    <row r="74" spans="1:5" ht="29">
-      <c r="A74" s="5" t="s">
+      <c r="E76" s="8"/>
+    </row>
+    <row r="77" spans="1:5" ht="29">
+      <c r="A77" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B74" s="18" t="s">
+      <c r="B77" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D77" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="E74" s="8"/>
-    </row>
-    <row r="75" spans="1:5" ht="57">
-      <c r="A75" s="5" t="s">
+      <c r="E77" s="8"/>
+    </row>
+    <row r="78" spans="1:5" ht="57">
+      <c r="A78" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B75" s="19" t="s">
+      <c r="B78" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D75" s="22" t="s">
+      <c r="D78" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="E75" s="14"/>
-    </row>
-    <row r="76" spans="1:5" ht="127">
-      <c r="A76" s="5" t="s">
+      <c r="E78" s="14"/>
+    </row>
+    <row r="79" spans="1:5" ht="127">
+      <c r="A79" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B76" s="19" t="s">
+      <c r="B79" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C79" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D79" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E76" s="8"/>
-    </row>
-    <row r="77" spans="1:5" ht="165">
-      <c r="A77" s="5" t="s">
+      <c r="E79" s="8"/>
+    </row>
+    <row r="80" spans="1:5" ht="165">
+      <c r="A80" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B80" s="9" t="s">
         <v>229</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="409.6">
-      <c r="A78" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="8" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="43">
-      <c r="A79" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="E79" s="8"/>
-    </row>
-    <row r="80" spans="1:5" ht="225">
-      <c r="A80" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>238</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D80" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="409.6">
+      <c r="A81" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="43">
+      <c r="A82" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E82" s="8"/>
+    </row>
+    <row r="83" spans="1:5" ht="225">
+      <c r="A83" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="E80" s="8" t="s">
+      <c r="E83" s="8" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="225">
-      <c r="A81" s="5" t="s">
+    <row r="84" spans="1:5" ht="225">
+      <c r="A84" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B84" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D84" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="E81" s="8" t="s">
+      <c r="E84" s="8" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="195">
-      <c r="A82" s="5" t="s">
+    <row r="85" spans="1:5" ht="195">
+      <c r="A85" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B85" s="10" t="s">
         <v>243</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D82" s="5"/>
-      <c r="E82" s="8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="370">
-      <c r="A83" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D83" s="5"/>
-      <c r="E83" s="8" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="300">
-      <c r="A84" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D84" s="5"/>
-      <c r="E84" s="8" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="328">
-      <c r="A85" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>253</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>244</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="328">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="370">
       <c r="A86" s="5" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>244</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="15">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="300">
       <c r="A87" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>259</v>
+        <v>249</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>250</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E87" s="8"/>
-    </row>
-    <row r="88" spans="1:5" ht="57">
+        <v>244</v>
+      </c>
+      <c r="D87" s="5"/>
+      <c r="E87" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="328">
       <c r="A88" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="E88" s="8"/>
-    </row>
-    <row r="89" spans="1:5" ht="165">
+        <v>244</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="328">
       <c r="A89" s="5" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="8" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="225">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15">
       <c r="A90" s="5" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="342">
+        <v>49</v>
+      </c>
+      <c r="E90" s="8"/>
+    </row>
+    <row r="91" spans="1:5" ht="57">
       <c r="A91" s="5" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="D91" s="5"/>
-      <c r="E91" s="8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="240">
+        <v>260</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E91" s="8"/>
+    </row>
+    <row r="92" spans="1:5" ht="165">
       <c r="A92" s="5" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="8" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="15">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="225">
       <c r="A93" s="5" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E93" s="8"/>
-    </row>
-    <row r="94" spans="1:5" ht="105">
+        <v>386</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="342">
       <c r="A94" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>281</v>
+        <v>270</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>271</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="60">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="240">
       <c r="A95" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>284</v>
+        <v>273</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>274</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="8" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="180">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15">
       <c r="A96" s="5" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="D96" s="5"/>
-      <c r="E96" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="165">
+        <v>278</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E96" s="8"/>
+    </row>
+    <row r="97" spans="1:5" ht="105">
       <c r="A97" s="5" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D97" s="5"/>
       <c r="E97" s="8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="285">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="60">
       <c r="A98" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>294</v>
+        <v>283</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>284</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>278</v>
       </c>
       <c r="D98" s="5"/>
       <c r="E98" s="8" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="135">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="180">
       <c r="A99" s="5" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="8" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="384">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="165">
       <c r="A100" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="B100" s="20" t="s">
-        <v>300</v>
+        <v>290</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>291</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="D100" s="5"/>
       <c r="E100" s="8" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="180">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="285">
       <c r="A101" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>304</v>
+        <v>293</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>294</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D101" s="5" t="s">
-        <v>388</v>
-      </c>
+      <c r="D101" s="5"/>
       <c r="E101" s="8" t="s">
-        <v>387</v>
+        <v>295</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="135">
       <c r="A102" s="5" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>278</v>
       </c>
       <c r="D102" s="5"/>
       <c r="E102" s="8" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="57">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="384">
       <c r="A103" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="B103" s="10" t="s">
-        <v>309</v>
+        <v>299</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>300</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="E103" s="8"/>
-    </row>
-    <row r="104" spans="1:5" ht="225">
+        <v>301</v>
+      </c>
+      <c r="D103" s="5"/>
+      <c r="E103" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="180">
       <c r="A104" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B104" s="10" t="s">
-        <v>313</v>
+        <v>303</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>304</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D104" s="5"/>
+      <c r="D104" s="5" t="s">
+        <v>388</v>
+      </c>
       <c r="E104" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="150">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="135">
       <c r="A105" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="B105" s="20" t="s">
-        <v>316</v>
+        <v>305</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>306</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>317</v>
+        <v>278</v>
       </c>
       <c r="D105" s="5"/>
       <c r="E105" s="8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="285">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="57">
       <c r="A106" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="B106" s="9" t="s">
-        <v>240</v>
+        <v>308</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>309</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="D106" s="5"/>
-      <c r="E106" s="8" t="s">
-        <v>321</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="E106" s="8"/>
     </row>
     <row r="107" spans="1:5" ht="225">
       <c r="A107" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="B107" s="20" t="s">
-        <v>323</v>
+        <v>312</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>313</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>390</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="D107" s="5"/>
       <c r="E107" s="8" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="43">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="150">
       <c r="A108" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="B108" s="10" t="s">
-        <v>209</v>
+        <v>315</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>316</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="E108" s="8"/>
-    </row>
-    <row r="109" spans="1:5" ht="150">
+        <v>317</v>
+      </c>
+      <c r="D108" s="5"/>
+      <c r="E108" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="285">
       <c r="A109" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="B109" s="10" t="s">
-        <v>328</v>
+        <v>319</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>240</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="D109" s="5"/>
       <c r="E109" s="8" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="240">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="225">
       <c r="A110" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="B110" s="10" t="s">
-        <v>331</v>
+        <v>322</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>323</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="180">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="43">
       <c r="A111" s="5" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>333</v>
+        <v>209</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>326</v>
       </c>
       <c r="D111" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="E111" s="8"/>
+    </row>
+    <row r="112" spans="1:5" ht="150">
+      <c r="A112" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="D112" s="5"/>
+      <c r="E112" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="240">
+      <c r="A113" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B113" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="180">
+      <c r="A114" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="D114" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="E111" s="8" t="s">
+      <c r="E114" s="8" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="239">
-      <c r="A112" s="5" t="s">
+    <row r="115" spans="1:5" ht="239">
+      <c r="A115" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="B115" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="C115" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="D115" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="E112" s="8"/>
-    </row>
-    <row r="113" spans="1:5" ht="14">
-      <c r="A113" s="7"/>
-      <c r="B113" s="7"/>
-      <c r="C113" s="7"/>
-      <c r="D113" s="7"/>
-      <c r="E113" s="21"/>
-    </row>
-    <row r="114" spans="1:5" ht="14">
-      <c r="A114" s="7"/>
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="7"/>
-      <c r="E114" s="21"/>
-    </row>
-    <row r="115" spans="1:5" ht="14">
-      <c r="A115" s="7"/>
-      <c r="B115" s="7"/>
-      <c r="C115" s="7"/>
-      <c r="D115" s="7"/>
-      <c r="E115" s="21"/>
+      <c r="E115" s="8"/>
     </row>
     <row r="116" spans="1:5" ht="14">
       <c r="A116" s="7"/>
@@ -11071,6 +11194,27 @@
       <c r="C1032" s="7"/>
       <c r="D1032" s="7"/>
       <c r="E1032" s="21"/>
+    </row>
+    <row r="1033" spans="1:5" ht="14">
+      <c r="A1033" s="7"/>
+      <c r="B1033" s="7"/>
+      <c r="C1033" s="7"/>
+      <c r="D1033" s="7"/>
+      <c r="E1033" s="21"/>
+    </row>
+    <row r="1034" spans="1:5" ht="14">
+      <c r="A1034" s="7"/>
+      <c r="B1034" s="7"/>
+      <c r="C1034" s="7"/>
+      <c r="D1034" s="7"/>
+      <c r="E1034" s="21"/>
+    </row>
+    <row r="1035" spans="1:5" ht="14">
+      <c r="A1035" s="7"/>
+      <c r="B1035" s="7"/>
+      <c r="C1035" s="7"/>
+      <c r="D1035" s="7"/>
+      <c r="E1035" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -11130,51 +11274,54 @@
     <hyperlink ref="B69" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
     <hyperlink ref="B70" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
     <hyperlink ref="B71" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B72" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B73" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B74" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B75" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B76" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B77" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B78" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B79" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B80" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B81" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B82" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B83" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B84" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B85" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B86" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B87" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B88" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B89" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B90" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B91" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B92" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B93" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B94" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="B95" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="B96" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B97" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="B98" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="B99" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="B100" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="B101" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="B102" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="B103" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="B104" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="B105" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="B106" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="B107" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="B108" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="B109" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="B110" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="B111" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="B112" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B74" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B76" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B77" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B78" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B79" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B80" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B81" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B82" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B83" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B84" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B85" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B86" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B87" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B88" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B89" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B90" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B91" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B92" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B93" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B94" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B95" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B96" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B97" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B98" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B99" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B100" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B101" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B102" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B103" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B104" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B105" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B106" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B107" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B108" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B109" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B110" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B111" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B112" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B113" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B114" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B115" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
     <hyperlink ref="B28" r:id="rId98" xr:uid="{3E36E18E-D7E1-0E43-BA0F-87728CDAE7F5}"/>
     <hyperlink ref="B25" r:id="rId99" xr:uid="{051F61AE-5CD5-724E-BEE6-AF148A6088D1}"/>
     <hyperlink ref="D44" r:id="rId100" xr:uid="{7F191D76-E8E5-C644-803F-C303BDB3A45A}"/>
-    <hyperlink ref="D75" r:id="rId101" xr:uid="{64084E7D-3DBE-994A-B04B-5B4E1461966B}"/>
+    <hyperlink ref="D78" r:id="rId101" xr:uid="{64084E7D-3DBE-994A-B04B-5B4E1461966B}"/>
+    <hyperlink ref="B75" r:id="rId102" xr:uid="{7E4E6CC0-3E4E-614A-B243-1348E92BA80D}"/>
+    <hyperlink ref="B72" r:id="rId103" xr:uid="{2EA8B205-AD96-3046-BAAD-6B74E2609355}"/>
+    <hyperlink ref="B73" r:id="rId104" xr:uid="{14818CE1-225F-2F41-BDA9-444BD7782FB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
open target in new tab
</commit_message>
<xml_diff>
--- a/Leetcode_Approach.xlsx
+++ b/Leetcode_Approach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunwsingh/Projects/coding-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216E15EA-1AE8-5F4D-9D5A-B3D7FB3F55E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ECA327-F82D-F240-9F30-124062057A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,9 +535,6 @@
   </si>
   <si>
     <t>Find Duplicate</t>
-  </si>
-  <si>
-    <t>mark num[num[i]] as -1, if already negative again it is duplicate</t>
   </si>
   <si>
     <t>Move Zeroes</t>
@@ -2729,6 +2726,9 @@
         }
         return cnt;
     }</t>
+  </si>
+  <si>
+    <t>Mark num[num[i]] as -1, if already negative again it is duplicate</t>
   </si>
 </sst>
 </file>
@@ -3160,8 +3160,8 @@
   </sheetPr>
   <dimension ref="A1:F1037"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B109" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="210">
@@ -3345,7 +3345,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>40</v>
@@ -3362,10 +3362,10 @@
         <v>43</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="342">
@@ -3379,10 +3379,10 @@
         <v>43</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>406</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="29">
@@ -3408,13 +3408,13 @@
         <v>50</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="398">
@@ -3445,10 +3445,10 @@
         <v>43</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="370">
@@ -3462,7 +3462,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>60</v>
@@ -3535,1038 +3535,1038 @@
         <v>75</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="8" t="s">
-        <v>76</v>
-      </c>
+      <c r="D25" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="180">
       <c r="A26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>78</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="105">
       <c r="A27" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="135">
       <c r="A28" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="225">
       <c r="A29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="180">
       <c r="A30" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>87</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="225">
       <c r="A31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="370">
       <c r="A32" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>93</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="180">
       <c r="A33" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="29">
       <c r="A34" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="C34" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="D34" s="12" t="s">
         <v>99</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>100</v>
       </c>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="180">
       <c r="A35" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="C35" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>103</v>
-      </c>
       <c r="D35" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="180">
       <c r="A36" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>105</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="195">
       <c r="A37" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="C37" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="90">
       <c r="A38" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="C38" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="120">
       <c r="A39" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>114</v>
-      </c>
       <c r="C39" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="409.6">
       <c r="A40" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="C40" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>118</v>
-      </c>
       <c r="E40" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="120">
       <c r="A41" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="C41" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="120">
       <c r="A42" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="C42" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="135">
       <c r="A43" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="C43" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="43">
       <c r="A44" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="C44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="22" t="s">
         <v>128</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="E44" s="14"/>
     </row>
     <row r="45" spans="1:5" ht="210">
       <c r="A45" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>131</v>
-      </c>
       <c r="C45" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="225">
       <c r="A46" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="C46" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="29">
       <c r="A47" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>135</v>
-      </c>
       <c r="C47" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="398">
       <c r="A48" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="B48" s="10" t="s">
-        <v>137</v>
-      </c>
       <c r="C48" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="113">
       <c r="A49" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="C49" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" ht="409.6">
       <c r="A50" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="C50" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15">
       <c r="A51" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>146</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="57">
       <c r="A52" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B52" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="C52" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="15" t="s">
         <v>149</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>150</v>
       </c>
       <c r="E52" s="16"/>
     </row>
     <row r="53" spans="1:5" ht="314">
       <c r="A53" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="C53" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>153</v>
       </c>
       <c r="D53" s="17"/>
       <c r="E53" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="409.6">
       <c r="A54" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>156</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="195">
       <c r="A55" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>158</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>159</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="29">
       <c r="A56" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="C56" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>164</v>
       </c>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="165">
       <c r="A57" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>166</v>
-      </c>
       <c r="C57" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="85">
       <c r="A58" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="C58" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="D58" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>170</v>
       </c>
       <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" ht="408" customHeight="1">
       <c r="A59" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="C59" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="D59" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="225">
       <c r="A60" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="C60" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="E60" s="8"/>
     </row>
     <row r="61" spans="1:5" ht="71">
       <c r="A61" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B61" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="C61" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="E61" s="8"/>
     </row>
     <row r="62" spans="1:5" ht="370">
       <c r="A62" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B62" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="B62" s="10" t="s">
-        <v>181</v>
-      </c>
       <c r="C62" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="165">
       <c r="A63" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B63" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="C63" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="342">
       <c r="A64" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="C64" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>189</v>
-      </c>
       <c r="D64" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="E64" s="8" t="s">
         <v>371</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="240">
       <c r="A65" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="B65" s="10" t="s">
-        <v>191</v>
-      </c>
       <c r="C65" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="29">
       <c r="A66" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="C66" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="E66" s="8"/>
     </row>
     <row r="67" spans="1:5" ht="270">
       <c r="A67" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B67" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="B67" s="10" t="s">
-        <v>196</v>
-      </c>
       <c r="C67" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="409.6">
       <c r="A68" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B68" s="22" t="s">
         <v>410</v>
       </c>
-      <c r="B68" s="22" t="s">
+      <c r="C68" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="D68" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="E68" s="21" t="s">
         <v>413</v>
-      </c>
-      <c r="E68" s="21" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="135">
       <c r="A69" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="197">
       <c r="A70" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B70" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="C70" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D70" s="12" t="s">
         <v>201</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>202</v>
       </c>
       <c r="E70" s="13"/>
     </row>
     <row r="71" spans="1:5" ht="29">
       <c r="A71" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B71" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="C71" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D71" s="12" t="s">
         <v>204</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>205</v>
       </c>
       <c r="E71" s="8"/>
     </row>
     <row r="72" spans="1:5" ht="165">
       <c r="A72" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B72" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="C72" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>208</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="280" customHeight="1">
       <c r="A73" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>399</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D73" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="B73" s="22" t="s">
-        <v>400</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>402</v>
-      </c>
       <c r="E73" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="409" customHeight="1">
       <c r="A74" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="C74" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="B74" s="22" t="s">
-        <v>403</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>405</v>
-      </c>
       <c r="D74" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E74" s="21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="85">
       <c r="A75" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B75" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="C75" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D75" s="12" t="s">
         <v>211</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>212</v>
       </c>
       <c r="E75" s="8"/>
     </row>
     <row r="76" spans="1:5" ht="285">
       <c r="A76" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="B76" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="B76" s="23" t="s">
+      <c r="C76" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="E76" s="21" t="s">
         <v>396</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="E76" s="21" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="225">
       <c r="A77" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B77" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="C77" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="E77" s="8"/>
     </row>
     <row r="78" spans="1:5" ht="29">
       <c r="A78" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B78" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="B78" s="18" t="s">
+      <c r="C78" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="E78" s="8"/>
     </row>
     <row r="79" spans="1:5" ht="57">
       <c r="A79" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B79" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="B79" s="19" t="s">
+      <c r="C79" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="D79" s="22" t="s">
         <v>221</v>
-      </c>
-      <c r="D79" s="22" t="s">
-        <v>222</v>
       </c>
       <c r="E79" s="14"/>
     </row>
     <row r="80" spans="1:5" ht="127">
       <c r="A80" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B80" s="19" t="s">
         <v>223</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>224</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E80" s="8"/>
     </row>
     <row r="81" spans="1:5" ht="165">
       <c r="A81" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B81" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>227</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="409.6">
       <c r="A82" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B82" s="10" t="s">
         <v>228</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>229</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="43">
       <c r="A83" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B83" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="C83" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="D83" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>234</v>
       </c>
       <c r="E83" s="8"/>
     </row>
     <row r="84" spans="1:5" ht="225">
       <c r="A84" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B84" s="9" t="s">
         <v>235</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>236</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="225">
       <c r="A85" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B85" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="B85" s="10" t="s">
+      <c r="C85" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C85" s="5" t="s">
-        <v>239</v>
-      </c>
       <c r="D85" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="E85" s="8" t="s">
         <v>381</v>
-      </c>
-      <c r="E85" s="8" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="195">
       <c r="A86" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B86" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="C86" s="5" t="s">
         <v>241</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>242</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="370">
       <c r="A87" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B87" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="B87" s="10" t="s">
-        <v>245</v>
-      </c>
       <c r="C87" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="300">
       <c r="A88" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B88" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B88" s="10" t="s">
-        <v>248</v>
-      </c>
       <c r="C88" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="328">
       <c r="A89" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B89" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="B89" s="10" t="s">
-        <v>251</v>
-      </c>
       <c r="C89" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="328">
       <c r="A90" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B90" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="B90" s="10" t="s">
-        <v>254</v>
-      </c>
       <c r="C90" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="15">
       <c r="A91" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="C91" s="5" t="s">
         <v>257</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>258</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>48</v>
@@ -4575,403 +4575,403 @@
     </row>
     <row r="92" spans="1:5" ht="57">
       <c r="A92" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B92" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="B92" s="10" t="s">
+      <c r="C92" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="E92" s="8"/>
     </row>
     <row r="93" spans="1:5" ht="165">
       <c r="A93" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B93" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="B93" s="10" t="s">
-        <v>263</v>
-      </c>
       <c r="C93" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="225">
       <c r="A94" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B94" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="C94" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C94" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="D94" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="342">
       <c r="A95" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B95" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="B95" s="10" t="s">
-        <v>269</v>
-      </c>
       <c r="C95" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="240">
       <c r="A96" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B96" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="B96" s="10" t="s">
-        <v>272</v>
-      </c>
       <c r="C96" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D96" s="5"/>
       <c r="E96" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15">
       <c r="A97" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B97" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="B97" s="9" t="s">
+      <c r="C97" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="D97" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="E97" s="8"/>
     </row>
     <row r="98" spans="1:5" ht="105">
       <c r="A98" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B98" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="B98" s="9" t="s">
-        <v>279</v>
-      </c>
       <c r="C98" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D98" s="5"/>
       <c r="E98" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="60">
       <c r="A99" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B99" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="B99" s="9" t="s">
-        <v>282</v>
-      </c>
       <c r="C99" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="180">
       <c r="A100" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B100" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="C100" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="D100" s="5"/>
       <c r="E100" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="165">
       <c r="A101" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B101" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="B101" s="9" t="s">
-        <v>289</v>
-      </c>
       <c r="C101" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D101" s="5"/>
       <c r="E101" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="285">
       <c r="A102" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B102" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="B102" s="10" t="s">
-        <v>292</v>
-      </c>
       <c r="C102" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D102" s="5"/>
       <c r="E102" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="135">
       <c r="A103" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B103" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="B103" s="9" t="s">
-        <v>295</v>
-      </c>
       <c r="C103" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D103" s="5"/>
       <c r="E103" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="384">
       <c r="A104" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B104" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="B104" s="20" t="s">
+      <c r="C104" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="D104" s="5"/>
       <c r="E104" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="180">
       <c r="A105" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B105" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="B105" s="9" t="s">
-        <v>302</v>
-      </c>
       <c r="C105" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="135">
       <c r="A106" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B106" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="B106" s="9" t="s">
-        <v>304</v>
-      </c>
       <c r="C106" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D106" s="5"/>
       <c r="E106" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="57">
       <c r="A107" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B107" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="B107" s="10" t="s">
+      <c r="C107" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="D107" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>309</v>
       </c>
       <c r="E107" s="8"/>
     </row>
     <row r="108" spans="1:5" ht="225">
       <c r="A108" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B108" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="B108" s="10" t="s">
-        <v>311</v>
-      </c>
       <c r="C108" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D108" s="5"/>
       <c r="E108" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="150">
       <c r="A109" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B109" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="B109" s="20" t="s">
+      <c r="C109" s="5" t="s">
         <v>314</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>315</v>
       </c>
       <c r="D109" s="5"/>
       <c r="E109" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="255">
       <c r="A110" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="B110" s="24" t="s">
         <v>415</v>
-      </c>
-      <c r="B110" s="24" t="s">
-        <v>416</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D110" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="E110" s="21" t="s">
         <v>417</v>
-      </c>
-      <c r="E110" s="21" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="285">
       <c r="A111" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C111" s="5" t="s">
         <v>317</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>318</v>
       </c>
       <c r="D111" s="5"/>
       <c r="E111" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="225">
       <c r="A112" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B112" s="20" t="s">
         <v>320</v>
       </c>
-      <c r="B112" s="20" t="s">
+      <c r="C112" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="C112" s="5" t="s">
-        <v>322</v>
-      </c>
       <c r="D112" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="43">
       <c r="A113" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B113" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C113" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="B113" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>324</v>
-      </c>
       <c r="D113" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E113" s="8"/>
     </row>
     <row r="114" spans="1:5" ht="150">
       <c r="A114" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B114" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="B114" s="10" t="s">
-        <v>326</v>
-      </c>
       <c r="C114" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D114" s="5"/>
       <c r="E114" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="240">
       <c r="A115" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B115" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="B115" s="10" t="s">
-        <v>329</v>
-      </c>
       <c r="C115" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="180">
       <c r="A116" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B116" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="B116" s="10" t="s">
-        <v>331</v>
-      </c>
       <c r="C116" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D116" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="E116" s="8" t="s">
         <v>391</v>
-      </c>
-      <c r="E116" s="8" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="239">
       <c r="A117" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B117" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="B117" s="10" t="s">
+      <c r="C117" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="C117" s="5" t="s">
+      <c r="D117" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>335</v>
       </c>
       <c r="E117" s="8"/>
     </row>

</xml_diff>

<commit_message>
read data from published sheet
</commit_message>
<xml_diff>
--- a/Leetcode_Approach.xlsx
+++ b/Leetcode_Approach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunwsingh/Projects/coding-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE64681-E5A9-EA4A-98AC-5563810C1C8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2466C25D-7426-CF45-A1CD-6AADBCB80BE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1924,16 +1924,6 @@
                 tailTable[CeilIndex(tailTable, -1, len - 1, A[i])] = A[i]; 
         } 
         return len; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    
-        if (i == 0 || j == 0)  
-            L[i][j] = 0;  
-        else if (X[i - 1] == Y[j - 1])  
-            L[i][j] = L[i - 1][j - 1] + 1;  
-        else
-            L[i][j] = max(L[i - 1][j], L[i][j - 1]);  
-        }  </t>
   </si>
   <si>
     <t>L[I][j] = LCS for X[0..I-1] and Y[0..j-1]</t>
@@ -2091,15 +2081,6 @@
     <t>Use Topological sort with dfs.
 1. Build adjacency list
 2. Do Topological sort for all characters. If already visited, return blank as there is a cycle N = 26;</t>
-  </si>
-  <si>
-    <t>DP:
-Sort by start times
-dp[I] represents total non overlapping intervals unto I
-dp[i] = max(dp[j]) + 1 0 &lt;= j &lt; I
-Greedy:
-{all intervals} - {max compatible intervals} = minimum deleted intervals
-Sort by end  times, to choose the smaller interval as we will be picking an interval ending earlier.</t>
   </si>
   <si>
     <t>// dp
@@ -3434,30 +3415,89 @@
 dp(S) = min {dp(S−ci)}+1, where i=0...n−1</t>
   </si>
   <si>
-    <t xml:space="preserve">    public int coinChange(int[] coins, int amount) {
-        if(amount==0)
-            return 0;
-        int n = Max_InT;
-        for(int coin : coins) {
-            int curr = 0;
-            if (amount &gt;= coin) {
-                int next = coinChange(coins, amount-coin);
-                if(next &gt;= 0)
-                    curr = 1+next;
-            }
-            if(curr &gt; 0)
-                n = Math.min(n,curr);
+    <t>public int coinChange(int[] coins, int amount) {
+    if(amount==0)
+        return 0;
+    int n = Max_InT;
+    for(int coin : coins) {
+        int curr = 0;
+        if (amount &gt;= coin) {
+            int next = coinChange(coins, amount-coin);
+            if(next &gt;= 0)
+                curr = 1+next;
         }
-        int finalCount = (n==Max_InT) ? -1 : n;
-        return finalCount;
+        if(curr &gt; 0)
+            n = Math.min(n,curr);
     }
-        for (int i = 1; i &lt;= amount; i++) {
-            for (int coin: coins) {
-                if (i - coin &gt;= 0) {
-                    dp[i] = Math.min(dp[i], dp[i - coin] + 1);
-                }
-            }
-        }</t>
+    int finalCount = (n==Max_InT) ? -1 : n;
+    return finalCount;
+}
+init dp array with int_max and dp[0] = 0
+for (int i = 1; i &lt;= amount; i++) {
+    for (int coin: coins) {
+        if (i - coin &gt;= 0) {
+            dp[i] = Math.min(dp[i], dp[i - coin] + 1);
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t>// time complexity - O(2^(m+n))
+// space complexity - O(m+n)
+public static int LCSM1(char[] X, char[] Y, int i, int j) {
+	if (i &lt;= 0 || j &lt;= 0)
+		return 0;
+	if (X[i - 1] == Y[j - 1])
+		return 1 + LCSM1(X, Y, i - 1, j - 1);
+	else
+		return Math.max(LCSM1(X, Y, i, j - 1), LCSM1(X, Y, i - 1, j));
+}
+// Recursive solution with memoization
+// time complexity - O(m*n)
+// space complexity - O(m*n)
+public static int LCSM2(char[] X, char[] Y, int i, int j, Integer[][] dp) {
+	if (i &lt;= 0 || j &lt;= 0)
+		return 0;
+	if (dp[i][j] != null)
+		return dp[i][j];
+	if (X[i - 1] == Y[j - 1])
+		return 1 + LCSM2(X, Y, i - 1, j - 1, dp);
+	else
+		return dp[i][j] = Math.max(LCSM2(X, Y, i, j - 1, dp), LCSM2(X, Y, i - 1, j, dp));
+}
+// Method3()- DP solution(Bottom up approach)
+// time complexity - O(m*n)
+// space complexity - O(m*n)
+public static int LCSM3(char[] X, char[] Y, int m, int n) {
+	int memo[][] = new int[m + 1][n + 1];
+	for (int i = 0; i &lt;= m; i++) {
+		for (int j = 0; j &lt;= n; j++) {
+			if (i == 0 || j == 0)
+				memo[i][j] = 0;
+			else if (X[i - 1] == Y[j - 1])
+				memo[i][j] = memo[i - 1][j - 1] + 1;
+			else
+				memo[i][j] = Math.max(memo[i - 1][j], memo[i][j - 1]);
+		}
+	}
+	return memo[m][n];
+}</t>
+  </si>
+  <si>
+    <t>we are trying to find max number of non overlapping intervals
+1. What if we sort by start date and remove subsequent intervals that overlapped with earliest interval
+Fails [1,8], [2,3], [4,5] as we will remove the smaller ones. So, we return 1 but the answer should have been 2
+2. What if we select the shortest interval:
+fails [1,5], [4,7], [6,8] as we will remove the bigger ones.
+This is why we sort by finishing time, so that we can pick max non overlapping intervals
+if we choose the interval that ends earlier, then there is more space for other intervals
+DP:
+Sort by start times
+dp[I] represents total non overlapping intervals unto I
+dp[i] = max(dp[j]) + 1 0 &lt;= j &lt; I
+Greedy:
+{all intervals} - {max compatible intervals} = minimum deleted intervals
+Sort by end  times, to choose the smaller interval as we will be picking an interval ending earlier.</t>
   </si>
 </sst>
 </file>
@@ -3889,8 +3929,8 @@
   </sheetPr>
   <dimension ref="A1:F1052"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
@@ -3956,7 +3996,7 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="210">
@@ -3980,7 +4020,7 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="8" t="s">
@@ -3989,16 +4029,16 @@
     </row>
     <row r="7" spans="1:6" ht="240">
       <c r="A7" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>469</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>470</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>471</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>20</v>
@@ -4006,36 +4046,36 @@
     </row>
     <row r="8" spans="1:6" ht="255">
       <c r="A8" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="D8" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>472</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>475</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="300">
       <c r="A9" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>480</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>481</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>475</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>483</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="285">
@@ -4044,7 +4084,7 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
@@ -4057,7 +4097,7 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="8" t="s">
@@ -4070,7 +4110,7 @@
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="8" t="s">
@@ -4083,7 +4123,7 @@
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="8" t="s">
@@ -4109,98 +4149,98 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="195">
       <c r="A16" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>438</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>439</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="409.6">
       <c r="A17" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>448</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>449</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="409.6">
       <c r="A18" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>453</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>454</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="225">
       <c r="A19" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="E19" s="21" t="s">
         <v>434</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>433</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="409.6">
       <c r="A20" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>443</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>447</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="150">
@@ -4222,53 +4262,53 @@
     </row>
     <row r="22" spans="1:5" ht="225">
       <c r="A22" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>456</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>457</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>458</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>460</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="356">
       <c r="A23" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="E23" s="21" t="s">
         <v>461</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>462</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>466</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="165">
       <c r="A24" s="7" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B24" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="E24" s="21" t="s">
         <v>465</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>468</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="342">
@@ -4279,13 +4319,13 @@
         <v>40</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="29">
@@ -4385,7 +4425,7 @@
         <v>58</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="85">
@@ -4414,10 +4454,10 @@
         <v>64</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="384">
@@ -4446,10 +4486,10 @@
         <v>38</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="180">
@@ -4653,7 +4693,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="356">
+    <row r="49" spans="1:5" ht="384">
       <c r="A49" s="5" t="s">
         <v>105</v>
       </c>
@@ -4664,27 +4704,27 @@
         <v>104</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="409.6">
       <c r="A50" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>104</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="409.6">
@@ -4706,22 +4746,22 @@
     </row>
     <row r="52" spans="1:5" ht="409.6">
       <c r="A52" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>104</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="120">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="409.6">
       <c r="A53" s="5" t="s">
         <v>111</v>
       </c>
@@ -4732,10 +4772,10 @@
         <v>109</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>344</v>
+        <v>488</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="120">
@@ -4749,10 +4789,10 @@
         <v>109</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="135">
@@ -4781,10 +4821,10 @@
         <v>104</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="210">
@@ -4798,10 +4838,10 @@
         <v>104</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="225">
@@ -4816,7 +4856,7 @@
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="29">
@@ -4831,7 +4871,7 @@
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="398">
@@ -4876,7 +4916,7 @@
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15">
@@ -4917,11 +4957,11 @@
         <v>143</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D65" s="17"/>
       <c r="E65" s="16" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="409.6">
@@ -4980,10 +5020,10 @@
         <v>153</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="85">
@@ -5012,27 +5052,27 @@
         <v>163</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="408" customHeight="1">
       <c r="A72" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="225">
@@ -5082,19 +5122,19 @@
     </row>
     <row r="76" spans="1:5" ht="409.6">
       <c r="A76" s="7" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>144</v>
       </c>
       <c r="D76" s="22" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="165">
@@ -5112,7 +5152,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="342">
+    <row r="78" spans="1:5" ht="409.6">
       <c r="A78" s="5" t="s">
         <v>177</v>
       </c>
@@ -5123,10 +5163,10 @@
         <v>179</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>357</v>
+        <v>489</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="240">
@@ -5140,10 +5180,10 @@
         <v>175</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="29">
@@ -5172,27 +5212,27 @@
         <v>175</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="409.6">
       <c r="A82" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>394</v>
+      </c>
+      <c r="C82" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="B82" s="22" t="s">
+      <c r="D82" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="E82" s="21" t="s">
         <v>397</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="E82" s="21" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="135">
@@ -5255,36 +5295,36 @@
     </row>
     <row r="87" spans="1:5" ht="280" customHeight="1">
       <c r="A87" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B87" s="22" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>314</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="409" customHeight="1">
       <c r="A88" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B88" s="22" t="s">
+        <v>387</v>
+      </c>
+      <c r="C88" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="D88" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="E88" s="21" t="s">
         <v>391</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="E88" s="21" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="85">
@@ -5304,19 +5344,19 @@
     </row>
     <row r="90" spans="1:5" ht="285">
       <c r="A90" s="12" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>188</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="225">
@@ -5390,10 +5430,10 @@
         <v>38</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="409.6">
@@ -5437,10 +5477,10 @@
         <v>38</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="225">
@@ -5454,10 +5494,10 @@
         <v>229</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="195">
@@ -5522,17 +5562,17 @@
     </row>
     <row r="104" spans="1:5" ht="255">
       <c r="A104" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B104" s="22" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="21" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="328">
@@ -5606,10 +5646,10 @@
         <v>257</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="342">
@@ -5773,10 +5813,10 @@
         <v>266</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="135">
@@ -5841,19 +5881,19 @@
     </row>
     <row r="125" spans="1:5" ht="409.6">
       <c r="A125" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B125" s="24" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E125" s="21" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="285">
@@ -5882,10 +5922,10 @@
         <v>312</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="43">
@@ -5899,7 +5939,7 @@
         <v>314</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E128" s="8"/>
     </row>
@@ -5929,10 +5969,10 @@
         <v>314</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E130" s="8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="180">
@@ -5946,10 +5986,10 @@
         <v>314</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="342">
@@ -5960,13 +6000,13 @@
         <v>323</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>324</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="14">

</xml_diff>